<commit_message>
docs(desarrollo): Actualiza avance en el sprint 3
</commit_message>
<xml_diff>
--- a/02 DESARROLLO/SCELS/03 DESARROLLO/SCELS-CP-015.xlsx
+++ b/02 DESARROLLO/SCELS/03 DESARROLLO/SCELS-CP-015.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\BAKATI-GROUP\02 DESARROLLO\SCELS\03 DESARROLLO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB61970-575E-4E78-80E8-A0FE7DD70792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E22CCA-4CD6-49F6-BCC0-ED5DB9CF6CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,12 +614,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEB7B17"/>
         <bgColor rgb="FFEB7B17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -715,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -876,9 +870,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1171,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2474,7 +2465,7 @@
         <f t="shared" ref="H35:H36" si="2">G35-F35-INT((G35-F35-WEEKDAY(G35)+1)/7)</f>
         <v>31</v>
       </c>
-      <c r="I35" s="31">
+      <c r="I35" s="27">
         <v>0</v>
       </c>
       <c r="J35" s="1"/>
@@ -2519,8 +2510,8 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="I36" s="58">
-        <v>0.05</v>
+      <c r="I36" s="27">
+        <v>1</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2551,7 +2542,7 @@
       <c r="F37" s="45"/>
       <c r="G37" s="45"/>
       <c r="H37" s="46"/>
-      <c r="I37" s="31">
+      <c r="I37" s="27">
         <v>0</v>
       </c>
       <c r="J37" s="1"/>
@@ -2596,7 +2587,7 @@
         <f t="shared" ref="H38:H43" si="3">G38-F38-INT((G38-F38-WEEKDAY(G38)+1)/7)</f>
         <v>5</v>
       </c>
-      <c r="I38" s="31">
+      <c r="I38" s="27">
         <v>0</v>
       </c>
       <c r="J38" s="1"/>
@@ -2641,7 +2632,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I39" s="31">
+      <c r="I39" s="27">
         <v>0</v>
       </c>
       <c r="J39" s="1"/>
@@ -2686,7 +2677,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I40" s="31">
+      <c r="I40" s="27">
         <v>0</v>
       </c>
       <c r="J40" s="1"/>
@@ -2731,7 +2722,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I41" s="31">
+      <c r="I41" s="27">
         <v>0</v>
       </c>
       <c r="J41" s="1"/>
@@ -2776,7 +2767,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="I42" s="31">
+      <c r="I42" s="27">
         <v>0</v>
       </c>
       <c r="J42" s="1"/>
@@ -2821,7 +2812,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="I43" s="31">
+      <c r="I43" s="27">
         <v>0</v>
       </c>
       <c r="J43" s="1"/>
@@ -2853,7 +2844,7 @@
       <c r="F44" s="45"/>
       <c r="G44" s="45"/>
       <c r="H44" s="46"/>
-      <c r="I44" s="31">
+      <c r="I44" s="27">
         <v>0</v>
       </c>
       <c r="J44" s="1"/>
@@ -2898,7 +2889,7 @@
         <f t="shared" ref="H45:H49" si="4">G45-F45-INT((G45-F45-WEEKDAY(G45)+1)/7)</f>
         <v>4</v>
       </c>
-      <c r="I45" s="31">
+      <c r="I45" s="27">
         <v>0</v>
       </c>
       <c r="J45" s="1"/>
@@ -2943,7 +2934,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I46" s="31">
+      <c r="I46" s="27">
         <v>0</v>
       </c>
       <c r="J46" s="1"/>
@@ -2988,7 +2979,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I47" s="31">
+      <c r="I47" s="27">
         <v>0</v>
       </c>
       <c r="J47" s="1"/>
@@ -3033,7 +3024,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I48" s="31">
+      <c r="I48" s="27">
         <v>0</v>
       </c>
       <c r="J48" s="1"/>
@@ -3078,7 +3069,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I49" s="31">
+      <c r="I49" s="27">
         <v>0</v>
       </c>
       <c r="J49" s="1"/>
@@ -3121,7 +3112,7 @@
       </c>
       <c r="I50" s="37">
         <f>AVERAGE(I35:I49)</f>
-        <v>3.3333333333333335E-3</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>

</xml_diff>